<commit_message>
Added If condition to handle expected counts
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,12 +454,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -481,12 +481,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -508,12 +508,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -535,12 +535,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -550,24 +550,24 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -577,24 +577,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -604,56 +604,56 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -670,71 +670,71 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -744,38 +744,2414 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>caacn</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Portland</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>orcmp</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Daneri Mortuary</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>cadan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Lane Memorial Funeral Home</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ormlm</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Springfield Memorial Funeral Home</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ormsm</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>cablo</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>Canby Funeral Chapel</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>orccf</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Cremation</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Lane Memorial Funeral Home</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ormlm</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>The Omega Society</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>caoms</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>caacn</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Portland</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>orcmp</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Lane Memorial Funeral Home</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ormlm</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
     </row>
-    <row r="15"/>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Springfield Memorial Funeral Home</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ormsm</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>cablo</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>caacn</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>caaed</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Portland</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>orcmp</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Springfield Memorial Funeral Home</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ormsm</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>The Omega Society</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>caoms</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Alpha Cremation Services</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ormac</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>caacn</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Molalla Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>orcmf</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>cablo</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>caaed</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Molalla Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>orcmf</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Springfield Memorial Funeral Home</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ormsm</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Portland</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>orcmp</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Alpha Cremation Services</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ormac</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Molalla Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>orcmf</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>caacn</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Murphy-Musgrove Funeral Home</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ormmm</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Molalla Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>orcmf</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>caaed</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>The Omega Society</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>caoms</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>cadll</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Springfield Memorial Funeral Home</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ormsm</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Molalla Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>orcmf</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Alpha Cremation Services</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ormac</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Murphy-Musgrove Funeral Home</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ormmm</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Salem</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>orcms</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>cadll</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Brusie Funeral Home</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>cabru</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Molalla Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>orcmf</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>caaed</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Murphy-Musgrove Funeral Home</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ormmm</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Salem</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>orcms</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Musgrove Family Mortuary</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ormwl</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>The Omega Society</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>caoms</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Alpha Cremation Services</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ormac</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>caacr</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>cadll</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Musgrove Family Mortuary</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>ormwl</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Brusie Funeral Home</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>cabru</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Musgrove Family Mortuary</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ormwl</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Salem</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>orcms</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Alpha Cremation Services</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ormac</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>The Omega Society</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>caoms</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Musgrove Family Mortuary</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>ormwl</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>cadll</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>caacr</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Brusie Funeral Home</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>cabru</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Musgrove Family Mortuary</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ormwl</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Salem</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>orcms</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>cadll</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>caacr</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Brusie Funeral Home</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>cabru</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Affordable Mortuary</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>cabam</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Musgrove Family Mortuary</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ormwl</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Affordable Mortuary</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>cabam</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Crown Cremation Services - Salem</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>orcms</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Brusie Funeral Home</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>cabru</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>cadll</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Ullrey Memorial Chapel</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>caulm</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Affordable Mortuary</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>cabam</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Brusie Funeral Home</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>cabru</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Ullrey Memorial Chapel</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>caulm</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Affordable Mortuary</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>cabam</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Ullrey Memorial Chapel</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>caulm</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Ullrey Memorial Chapel</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>caulm</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Affordable Mortuary</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>cabam</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Ullrey Memorial Chapel</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>caulm</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Affordable Mortuary</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>cabam</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Ullrey Memorial Chapel</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>caulm</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="103"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated If else logic
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,12 +454,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -469,24 +469,24 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -508,12 +508,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Tualatin</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>orcmt</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -523,24 +523,24 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -562,12 +562,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -577,24 +577,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -616,12 +616,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -643,12 +643,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -658,24 +658,24 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -685,24 +685,24 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -712,24 +712,24 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Tualatin</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>orcmt</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -739,7 +739,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -751,12 +751,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -778,12 +778,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -798,19 +798,19 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -820,51 +820,51 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -874,24 +874,24 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -901,51 +901,51 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -955,78 +955,78 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1063,56 +1063,56 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1122,19 +1122,19 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1144,56 +1144,56 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1203,19 +1203,19 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1225,29 +1225,29 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1257,46 +1257,46 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1306,24 +1306,24 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1333,29 +1333,29 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1365,29 +1365,29 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1399,17 +1399,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1436,17 +1436,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1463,56 +1463,56 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1522,61 +1522,61 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1588,39 +1588,39 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1630,105 +1630,105 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1738,78 +1738,78 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1819,24 +1819,24 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1846,29 +1846,29 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1878,19 +1878,19 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1900,24 +1900,24 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1939,39 +1939,39 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1981,51 +1981,51 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2035,24 +2035,24 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2089,24 +2089,24 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2116,51 +2116,51 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2170,29 +2170,29 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2202,19 +2202,19 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2224,29 +2224,29 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2256,46 +2256,46 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2317,66 +2317,66 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2386,24 +2386,24 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2425,93 +2425,93 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2533,12 +2533,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2548,24 +2548,24 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2587,12 +2587,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2629,29 +2629,29 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2661,19 +2661,19 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2683,24 +2683,24 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2710,24 +2710,24 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2749,12 +2749,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2764,24 +2764,24 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2791,78 +2791,78 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2884,17 +2884,17 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2904,46 +2904,46 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2953,24 +2953,24 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2992,12 +2992,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3007,51 +3007,51 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3073,12 +3073,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3088,24 +3088,24 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3127,31 +3127,463 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>caaed</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Daneri Mortuary</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>cadan</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Canby Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>orccf</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>caaed</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Daneri Mortuary</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>cadan</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>caaed</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Canby Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>orccf</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Daneri Mortuary</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>cadan</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>caaed</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
     </row>
-    <row r="103"/>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Canby Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>orccf</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Daneri Mortuary</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>cadan</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Canby Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>orccf</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Daneri Mortuary</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>cadan</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Canby Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>orccf</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Daneri Mortuary</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>cadan</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Canby Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>orccf</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="119"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Headless mode. Created separate keyword to handle active plan found popup and made additional check to skip it for the first time.
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,12 +454,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Tualatin</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>orcmt</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -469,24 +469,24 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -496,24 +496,24 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -535,12 +535,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -562,12 +562,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -589,12 +589,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -616,12 +616,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Tualatin</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>orcmt</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -631,24 +631,24 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -670,12 +670,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -685,24 +685,24 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -724,12 +724,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -751,12 +751,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -778,12 +778,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -793,24 +793,24 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -825,19 +825,19 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -847,24 +847,24 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -874,24 +874,24 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -901,29 +901,29 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -940,39 +940,39 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -987,105 +987,105 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1095,19 +1095,19 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1117,78 +1117,78 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1198,24 +1198,24 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1225,29 +1225,29 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1257,19 +1257,19 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1279,24 +1279,24 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1306,56 +1306,56 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1365,19 +1365,19 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1387,24 +1387,24 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1426,17 +1426,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1453,39 +1453,39 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1495,12 +1495,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1517,56 +1517,56 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1635,46 +1635,46 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1684,29 +1684,29 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1716,19 +1716,19 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1738,29 +1738,29 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1770,19 +1770,19 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1804,54 +1804,54 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1873,24 +1873,24 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1912,12 +1912,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1927,51 +1927,51 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1981,24 +1981,24 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2008,24 +2008,24 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2040,19 +2040,19 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2062,51 +2062,51 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2128,44 +2128,44 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2175,19 +2175,19 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2197,78 +2197,78 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2278,24 +2278,24 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2305,24 +2305,24 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2332,51 +2332,51 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2386,24 +2386,24 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2440,24 +2440,24 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2467,24 +2467,24 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2506,17 +2506,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2533,12 +2533,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2548,24 +2548,24 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2597,29 +2597,29 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2641,12 +2641,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2668,39 +2668,39 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2710,24 +2710,24 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2737,24 +2737,24 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2764,24 +2764,24 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2791,51 +2791,51 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2845,56 +2845,56 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -2938,66 +2938,66 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3007,24 +3007,24 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3034,24 +3034,24 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3061,24 +3061,24 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3088,12 +3088,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -3115,24 +3115,24 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3142,56 +3142,56 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3208,39 +3208,39 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3250,51 +3250,51 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3304,29 +3304,29 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3336,19 +3336,19 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3358,24 +3358,24 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3385,29 +3385,29 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3417,19 +3417,19 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3439,24 +3439,24 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3466,51 +3466,51 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3520,24 +3520,24 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3559,12 +3559,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3583,7 +3583,88 @@
         </is>
       </c>
     </row>
-    <row r="119"/>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="122"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added wait to complete page load when opening Storefront & visiting the location details page.
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,12 +454,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -481,12 +481,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Daneri Mortuary</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>cadan</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -496,24 +496,24 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -523,24 +523,24 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Tualatin</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>orcmt</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -550,24 +550,24 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -589,12 +589,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -616,12 +616,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -643,12 +643,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -658,12 +658,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -697,12 +697,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -712,24 +712,24 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -739,24 +739,24 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Tualatin</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>orcmt</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -766,24 +766,24 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -805,12 +805,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -847,24 +847,24 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -874,7 +874,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -901,24 +901,24 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -928,12 +928,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -967,12 +967,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -982,51 +982,51 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1036,24 +1036,24 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1075,12 +1075,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1090,78 +1090,78 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Tualatin</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>orcmt</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1171,51 +1171,51 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1237,39 +1237,39 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1291,39 +1291,39 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1345,12 +1345,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1360,29 +1360,29 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1399,12 +1399,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1414,24 +1414,24 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Tualatin</t>
+          <t>Crown Cremation Services - Portland</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>orcmt</t>
+          <t>orcmp</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1453,12 +1453,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Crown Cremation Services - Tualatin</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>orcmt</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1468,12 +1468,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1507,12 +1507,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1522,24 +1522,24 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1561,12 +1561,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1588,12 +1588,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1615,17 +1615,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1635,19 +1635,19 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>The Omega Society</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>caoms</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1657,24 +1657,24 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>caaed</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1684,24 +1684,24 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Springfield Memorial Funeral Home</t>
+          <t>Daneri Mortuary</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ormsm</t>
+          <t>cadan</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1716,19 +1716,19 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Portland</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>orcmp</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1738,24 +1738,24 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1777,12 +1777,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>caacn</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1792,24 +1792,24 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Springfield Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>ormsm</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1819,29 +1819,29 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1851,46 +1851,46 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Lane Memorial Funeral Home</t>
+          <t>Blue Oaks Cremation &amp; Burial Services</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ormlm</t>
+          <t>cablo</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1912,12 +1912,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Blue Oaks Cremation &amp; Burial Services</t>
+          <t>Affordable Cremation &amp; Funeral Center - North Sacramento</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>cablo</t>
+          <t>caacn</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1939,12 +1939,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Canby Funeral Chapel</t>
+          <t>The Omega Society</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>orccf</t>
+          <t>caoms</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1959,19 +1959,19 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Lane Memorial Funeral Home</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>ormlm</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1981,12 +1981,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -2020,39 +2020,39 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Canby Funeral Chapel</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>orccf</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2062,78 +2062,78 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>El Dorado Funeral &amp; Cremation Services - Placerville</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>caaed</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2143,24 +2143,24 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2170,24 +2170,24 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2197,24 +2197,24 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2236,22 +2236,22 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Alpha Cremation Services</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>ormac</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2263,17 +2263,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Alpha Cremation Services</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ormac</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2283,46 +2283,46 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2332,24 +2332,24 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Amador Hills Cremation &amp; Funeral Service</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>cadll</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2359,24 +2359,24 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2398,39 +2398,39 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2440,12 +2440,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -2479,66 +2479,66 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>caacr</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2548,24 +2548,24 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2575,24 +2575,24 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2602,24 +2602,24 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2629,12 +2629,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2656,24 +2656,24 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Crown Cremation Services - Salem</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>orcms</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2683,39 +2683,39 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -2749,12 +2749,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2764,51 +2764,51 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2818,51 +2818,51 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2872,29 +2872,29 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Crown Cremation Services - Salem</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>orcms</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2904,19 +2904,19 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Musgrove Family Mortuary</t>
+          <t>Affordable Cremation &amp; Funeral Service - Roseville</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>ormwl</t>
+          <t>caacr</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2926,24 +2926,24 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2953,51 +2953,51 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Ullrey Memorial Chapel</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>caulm</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3007,12 +3007,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3029,29 +3029,29 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3061,29 +3061,29 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3115,51 +3115,51 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Affordable Mortuary</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>cabam</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3169,24 +3169,24 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Amador Hills Cremation &amp; Funeral Service</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>cadll</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3196,29 +3196,29 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3235,17 +3235,17 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Murphy-Musgrove Funeral Home</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>ormmm</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3255,19 +3255,19 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3289,12 +3289,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Musgrove Family Mortuary</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>ormwl</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3304,29 +3304,29 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>No Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Ullrey Memorial Chapel</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>caulm</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Burial</t>
+          <t>Cremation</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3336,19 +3336,19 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Murphy-Musgrove Funeral Home</t>
+          <t>Molalla Funeral Chapel</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>ormmm</t>
+          <t>orcmf</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3370,12 +3370,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Molalla Funeral Chapel</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>orcmf</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3385,39 +3385,39 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Brusie Funeral Home</t>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>cabru</t>
+          <t>caacs</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Cremation</t>
+          <t>Burial</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>No Facilities</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3451,12 +3451,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Brusie Funeral Home</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>cabru</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3466,24 +3466,24 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>All</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+          <t>Affordable Mortuary</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>caacs</t>
+          <t>cabam</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3505,31 +3505,166 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
+          <t>Molalla Funeral Chapel</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>orcmf</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
           <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
+      <c r="B117" t="inlineStr">
         <is>
           <t>caacs</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Cremation</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Burial</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Affordable Mortuary</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>cabam</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
     </row>
-    <row r="117"/>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>No Facilities</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Affordable Cremation &amp; Funeral Center - South Sacramento</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>caacs</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Cremation</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="122"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>